<commit_message>
refactor: increase assurance type-safety
</commit_message>
<xml_diff>
--- a/support/assurance/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>ingest_session_issue_id</t>
   </si>
@@ -42,13 +42,37 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>55b85aad-7260-4431-883f-7d41ec2d4976</t>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+  </si>
+  <si>
+    <t>Structural</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has no workflow</t>
+  </si>
+  <si>
+    <t>support/assurance/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has no workflow</t>
+  </si>
+  <si>
+    <t>9f5496ef-85e3-4c2d-a626-d1701c1b517e</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -60,7 +84,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>350dfaaa-8fd0-44f3-afe4-d47fa695766d</t>
+    <t>dca6daec-9721-42ed-82b9-43db619cc21d</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +93,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>25f7c4b0-43d9-4eaf-b9ed-a187ca2c3e5f</t>
+    <t>a70d0353-1947-4eaf-a3f3-fefef8f46951</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +102,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>b7b4195d-63fb-40d0-8ff7-dda5c3fcf442</t>
+    <t>b0fae2fb-a7d7-407e-b2b0-4a4f4ff1bcdf</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +111,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>9f8fc4cd-367e-432b-affa-6fe0b1e67bf6</t>
+    <t>36d64901-b8b9-41fa-b276-fe6d3ab1ae50</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +120,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>8e06e7ea-196c-486e-b7e6-7b4f535eec2e</t>
+    <t>37cb75e4-0f81-4224-9b7a-3bf177d9e559</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +129,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>f049d1e6-2aa3-4a15-93a3-33cc5bca57ed</t>
+    <t>8f9d9a6b-f441-43e7-906f-ea5e98e8a88a</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +138,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>153e41e0-4a67-4fd3-af1f-087856d3371e</t>
+    <t>10b1e6f8-6005-453d-8407-a318259dba02</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +147,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>22e180a6-6225-48fe-84b7-1ed2bb1f806f</t>
+    <t>834ce794-a560-4165-89c1-431e5705d34f</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +156,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>a4e9a61d-a286-44fa-a432-2e720d47afb6</t>
+    <t>18b89a50-72d4-4af8-a8d6-d16ff759b55b</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +165,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>146fefee-4116-4a59-8088-01ceb9e1b716</t>
+    <t>b5c45442-d6a7-495a-85b1-f8096277834e</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +174,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>eeecfbc8-3dbf-4fc0-aeb4-49c0257f4209</t>
+    <t>4c2640a5-389e-4be9-b7f8-c0fe91f754a1</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +183,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>7b018870-eb0a-4d7d-a9ed-f44803279428</t>
+    <t>f986543b-fdfb-4783-b2b4-b3467fd4b327</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +192,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>4b4e5dd4-e3ba-4e15-9ef4-04e415f82617</t>
+    <t>6a6ada6d-19ea-46ad-9243-73220149093a</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +201,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>ad5bf60c-020d-4eb1-b1a1-77963de52973</t>
+    <t>ace7f024-1654-42d0-8dcf-de51c240813b</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +210,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>f05fc09f-5a14-4046-8c93-07590efbf2fb</t>
+    <t>69ea64e9-bacb-4d8a-877e-237519e018e6</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +219,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>930b1a02-88fb-4877-b29b-e23b11b23c37</t>
+    <t>8b7860cb-cc90-4206-94af-d23d7e6a6fa1</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +228,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>1cd964d1-a2c5-41c3-b1f5-99e6d4ed52c2</t>
+    <t>351bac81-55a5-4f9b-9278-a1eea4b4c76b</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +237,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>9a07efc3-7387-407d-b26b-d855f2d5e7fc</t>
+    <t>a2fef3ef-49ad-4927-98a3-d972a0d6f07e</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +246,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>183835d4-6a89-42bf-b776-7df1549912fd</t>
+    <t>4750ee31-19b8-425a-86e1-82038754991b</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +255,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>bf4668a9-d79d-4069-835e-b3ed8779facf</t>
+    <t>975d3ca8-81e3-43f2-9860-8f8bff05262f</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,45 +264,45 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
+  </si>
+  <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>support/assurance/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
+  </si>
+  <si>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+  </si>
+  <si>
     <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
   </si>
   <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>Structural</t>
-  </si>
-  <si>
-    <t>Sheet 'Admin_Demographic' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
-  </si>
-  <si>
-    <t>support/assurance/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>36aa52c0-be32-4342-9586-a42ecedd57b0</t>
   </si>
   <si>
     <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
   </si>
   <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
-  </si>
-  <si>
-    <t>Sheet 'Screening' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
-  </si>
-  <si>
-    <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
-  </si>
-  <si>
-    <t>591191c7-f693-5957-8734-ac87151ca981</t>
-  </si>
-  <si>
-    <t>Sheet 'QE_Admin_Data' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
-  </si>
-  <si>
-    <t>48ba172c-f200-4f49-af93-2eb9ca17ff18</t>
-  </si>
-  <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
-  </si>
-  <si>
     <t>Data Type Mismatch</t>
   </si>
   <si>
@@ -294,82 +318,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>71edb554-b527-4912-8fef-86a24ef2604d</t>
-  </si>
-  <si>
-    <t>544ad610-65dd-4789-a220-7aacb70c9e4a</t>
-  </si>
-  <si>
-    <t>777be274-39b6-4ff4-8f7d-7b723b1ccac6</t>
-  </si>
-  <si>
-    <t>5ac5ae1f-1d75-4ae5-92ef-c861ea45a2d2</t>
-  </si>
-  <si>
-    <t>d6f3fc1d-cfb5-4267-b192-4cab5718aa46</t>
-  </si>
-  <si>
-    <t>b4bf293e-cece-44c2-89d6-09195a5d207f</t>
-  </si>
-  <si>
-    <t>82dd954b-92e9-44c1-a06f-f4a5a1e4023e</t>
-  </si>
-  <si>
-    <t>010d4ec7-767f-447c-abf6-ab911c73690b</t>
-  </si>
-  <si>
-    <t>dd8089b7-63d9-437f-9d40-721fa6705b27</t>
-  </si>
-  <si>
-    <t>854fc9c6-6b43-49c7-8f9d-a14821ea94ab</t>
-  </si>
-  <si>
-    <t>8c361ca6-59ea-4bfc-8a03-350672c1c8b4</t>
-  </si>
-  <si>
-    <t>3f29740c-8c06-4aa9-98d8-47b1deaa08d3</t>
-  </si>
-  <si>
-    <t>054221be-a1d8-48ec-a8a5-a78bd2075ac7</t>
-  </si>
-  <si>
-    <t>ad66b301-d48a-4cfd-bc67-9ec362fe8c7c</t>
-  </si>
-  <si>
-    <t>55514463-ba96-4299-9bc9-076472485d85</t>
-  </si>
-  <si>
-    <t>deb2dbab-6d61-4e19-b4be-3f880b7f451b</t>
-  </si>
-  <si>
-    <t>9c0b52cd-fabe-4a73-ad84-c4c4e8b256c7</t>
-  </si>
-  <si>
-    <t>1ba65f8c-2686-4745-8bef-e125ef79e85f</t>
-  </si>
-  <si>
-    <t>2108a73f-e1b2-497a-8412-852ad4576875</t>
-  </si>
-  <si>
-    <t>933920a2-4879-4c43-bcdc-971966105699</t>
-  </si>
-  <si>
-    <t>ee9c87e9-51a5-4995-aa66-d982fbee3f06</t>
-  </si>
-  <si>
-    <t>f9110922-eb51-4ea5-a132-cd0831e2dcfd</t>
-  </si>
-  <si>
-    <t>e12b026d-18b6-48cb-93a9-f3ed7da7be8c</t>
-  </si>
-  <si>
-    <t>9a983214-015b-4e39-a2cf-c149be5292d6</t>
-  </si>
-  <si>
-    <t>05192103-b177-4201-bac9-93bc4c3856c7</t>
-  </si>
-  <si>
-    <t>ff7be3f5-f4a2-4375-8144-60bd9b1e71c2</t>
+    <t>aec22b42-faa3-44e6-8b84-13a2d95b1589</t>
+  </si>
+  <si>
+    <t>45290f0f-c142-48e2-8ccb-b4f1bfe424a4</t>
+  </si>
+  <si>
+    <t>0ab90623-fa20-4ca7-8bbe-56dd4b5fbd2e</t>
+  </si>
+  <si>
+    <t>7ae62be8-e9d9-4c78-b6f0-5c2b5a5e99a4</t>
+  </si>
+  <si>
+    <t>48559a3e-26ff-42d0-848c-1017e6802a57</t>
+  </si>
+  <si>
+    <t>42cddd34-2911-4c22-a893-e690f9f01bca</t>
+  </si>
+  <si>
+    <t>cb1469d1-96bf-43a5-b35c-0a9c5c848fbc</t>
+  </si>
+  <si>
+    <t>94f0044e-0b8d-4ebd-a012-beae729bfacb</t>
+  </si>
+  <si>
+    <t>ac500824-e038-4d6c-ba10-b6058ff98d43</t>
+  </si>
+  <si>
+    <t>b4f5a1b1-066b-4a9f-b91b-4d59d4e92b23</t>
+  </si>
+  <si>
+    <t>2215ca62-56f7-4cd5-97f0-640755cce34b</t>
+  </si>
+  <si>
+    <t>fdd8dc0d-f1af-45f2-ac77-c9effa29148c</t>
+  </si>
+  <si>
+    <t>f8fb5dfc-c128-44fa-847c-22328911d607</t>
+  </si>
+  <si>
+    <t>1701823f-d140-4190-804f-fe1faa92dbfb</t>
+  </si>
+  <si>
+    <t>86965f41-3337-4e97-9417-7921c6479001</t>
+  </si>
+  <si>
+    <t>242fbd39-edbc-4bd1-bd73-44e2e813eb08</t>
+  </si>
+  <si>
+    <t>9c05bb9c-e30d-4dbc-87cf-e5dbab33a002</t>
+  </si>
+  <si>
+    <t>947eded6-09d9-43cc-bf52-3496fa7a468e</t>
+  </si>
+  <si>
+    <t>889f7234-3c27-44a5-8968-edcc0502e4d3</t>
+  </si>
+  <si>
+    <t>f691efc6-6b25-40c4-b180-9b1f03c63ce4</t>
+  </si>
+  <si>
+    <t>d149c294-8e29-448a-ac58-62921e9c5a6c</t>
+  </si>
+  <si>
+    <t>0c4c7f70-8de5-433f-96f8-20c17f91b1ce</t>
+  </si>
+  <si>
+    <t>a8ef06dc-952a-4a38-9a3c-7cb133beb189</t>
+  </si>
+  <si>
+    <t>d5296d66-d9a7-4460-a96c-ab20c8f74a18</t>
+  </si>
+  <si>
+    <t>0a58c4ae-2fc3-40af-bc7a-2f8f1fb4ee30</t>
+  </si>
+  <si>
+    <t>a42bf442-81b7-4ca1-a966-409044557df2</t>
   </si>
 </sst>
 </file>
@@ -486,7 +510,7 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -498,16 +522,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
         <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -518,395 +542,395 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>80</v>
       </c>
     </row>
@@ -918,16 +942,16 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
         <v>83</v>
-      </c>
-      <c r="H24" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25">
@@ -941,71 +965,53 @@
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" t="s">
         <v>88</v>
-      </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" t="s">
-        <v>92</v>
-      </c>
-      <c r="I26" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
         <v>94</v>
       </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="H27" t="s">
         <v>88</v>
-      </c>
-      <c r="D27" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="28">
@@ -1016,721 +1022,779 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H28" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I28" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H29" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I29" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H30" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I31" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H32" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I32" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H33" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I33" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F34">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H34" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F35">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H35" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I35" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F36">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G36" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H36" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I36" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F37">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H37" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I37" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F38">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H38" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I38" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F39">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H39" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I39" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F40">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H40" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I40" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F41">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H41" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I41" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F42">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H42" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I42" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F43">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H43" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I43" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E44" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F44">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H44" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I44" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F45">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G45" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H45" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I45" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D46" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E46" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F46">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H46" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I46" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F47">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G47" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H47" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I47" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F48">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G48" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H48" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I48" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F49">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H49" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I49" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E50" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F50">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H50" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I50" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E51" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F51">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G51" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H51" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I51" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D52" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F52">
+        <v>25</v>
+      </c>
+      <c r="G52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52" t="s">
+        <v>100</v>
+      </c>
+      <c r="I52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53">
+        <v>26</v>
+      </c>
+      <c r="G53" t="s">
+        <v>99</v>
+      </c>
+      <c r="H53" t="s">
+        <v>100</v>
+      </c>
+      <c r="I53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54">
         <v>27</v>
       </c>
-      <c r="G52" t="s">
-        <v>91</v>
-      </c>
-      <c r="H52" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" t="s">
-        <v>93</v>
+      <c r="G54" t="s">
+        <v>99</v>
+      </c>
+      <c r="H54" t="s">
+        <v>100</v>
+      </c>
+      <c r="I54" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: separate biz logic from workflow
</commit_message>
<xml_diff>
--- a/support/assurance/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/results-test-e2e/diagnostics.xlsx
@@ -51,16 +51,16 @@
     <t>168a34c7-d043-5ec4-a84a-c961f1a301ef</t>
   </si>
   <si>
-    <t>Structural</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has no workflow</t>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
   </si>
   <si>
     <t>support/assurance/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
   </si>
   <si>
-    <t>6a8e58ce-1cf9-49f1-9fab-0dc6e5b5b165</t>
+    <t>600e7ff2-9270-400d-8f53-6d51336e9465</t>
   </si>
   <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
@@ -75,7 +75,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>a98f509b-683f-4e59-b669-f60ad1f39686</t>
+    <t>4bff53aa-7b63-4595-b6e2-cb82ff761a44</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -84,7 +84,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>11b6cdb6-a79a-4455-8378-61a3bb705b96</t>
+    <t>1f4e687b-9e62-4ca4-927d-8ce6dc6e17f6</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -93,7 +93,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>6b080001-f75d-4584-9127-9d03e730cf32</t>
+    <t>fd36ecf0-814f-41e6-8def-f827a6428343</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -102,7 +102,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>4f5ec29a-1e71-4720-9619-e76caa3709cd</t>
+    <t>762b8876-4f63-4507-ac44-273c69a61427</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -111,7 +111,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>f99357d4-1f92-4208-92be-9d1457c91767</t>
+    <t>eea1968f-0db9-4e34-894f-bd2993c09ba5</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -120,7 +120,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>2af759a1-f53d-4603-85ca-8885b129cf6c</t>
+    <t>704cd277-2933-4211-8df3-6f800fc8a696</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -129,7 +129,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>0105e6fb-37ae-4065-93bf-ad4906d8fd70</t>
+    <t>6f09fee0-ec02-4f2d-903a-8ea9eafff274</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -138,7 +138,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>052b9205-8acc-44dd-adf8-146dcb56ea65</t>
+    <t>939d0637-9ca8-4f34-96bc-28efa27f4ab7</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -147,7 +147,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>290ea667-a8fc-4bf0-a4ba-21e21e3ff730</t>
+    <t>7e063e1e-455e-48d3-88fe-c63abf5689c7</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -156,7 +156,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>8f976ede-4883-44ce-b171-aca7e42a8db0</t>
+    <t>d80091b3-65a5-46f5-be82-d4cf3a80edf6</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in ahc_hrsn_valid_01_screening.</t>
@@ -165,7 +165,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>ee0fbdfb-b710-4201-b062-ad3f33d5bdd9</t>
+    <t>db723cdf-9fb5-46bc-867d-9ad57519aaf7</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -174,7 +174,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>838b1f70-116f-4710-8862-beb9360ed65b</t>
+    <t>c7fab8de-a65d-4003-86e8-338cb19bc7a6</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -183,7 +183,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>9cfe7745-db99-47cb-b020-66e5c672e2aa</t>
+    <t>e1875632-9d0a-4280-9445-00c613b23b60</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -192,7 +192,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>b995e28e-2234-469a-ab48-7ef2ee4dafb7</t>
+    <t>1a57febc-ab7f-4f31-b5c7-b40f00433bd7</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -201,7 +201,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>dbb0845a-ff5c-4302-ab23-5395a1cc085e</t>
+    <t>f3b7d1bc-954c-4f78-9ddf-90ef8e827e0e</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -210,7 +210,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>8f28e736-1d6a-45e0-8343-b421963a0528</t>
+    <t>29d6b3d3-4c48-47b5-82a8-7fc98691af60</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -219,7 +219,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>3d8b3a54-fd5a-408d-8bc1-19d97a326e17</t>
+    <t>739dd110-ca51-4a69-9db9-ef56b93bdd0a</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -228,7 +228,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>9594d4e7-0431-4572-a97c-4d34dbdc7785</t>
+    <t>70348106-a609-4982-8ab1-fdcbc2b150b7</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -237,7 +237,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>b34bbf00-7b86-4ef5-b7c3-d48ffe05dee6</t>
+    <t>9576fff7-d45b-4a1e-b8ef-40ed9522167f</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -246,7 +246,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>aec00e60-4018-4214-abf1-5aa1058d64f4</t>
+    <t>c0466663-5296-4ee3-b347-bb6855b15c97</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -261,10 +261,10 @@
     <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
   </si>
   <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has no workflow</t>
-  </si>
-  <si>
-    <t>b95d7c3f-48c8-4274-aeb8-865297aaa770</t>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>5d3dbe64-c29e-4f0a-8ca3-5ee94778708c</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>931349ae-0e95-479f-ab5b-5db4e3580410</t>
+    <t>66d7eaa2-5042-47bf-8c88-2a23229b0bde</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>e3d26ecb-0868-49fa-baf7-816c9c3da61e</t>
+    <t>94da5182-eb64-4b8f-8392-96928cea41c2</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>a3eb149f-b3e1-4cb2-864c-586b061f529e</t>
+    <t>85adf558-1245-4354-a4f2-c1bee1af2821</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>bc99bec8-8b07-453a-b018-61a27a79de3a</t>
+    <t>178124f2-ecac-41d8-ab3a-1d5e14b53345</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>9df4104f-01c7-4dda-8ed5-1282dec0750b</t>
+    <t>0a5cc160-2382-4f7c-84bd-baa7a858a2b4</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>ccdb553c-c15c-49ce-822e-c1c2eb59b54e</t>
+    <t>b6b67033-0c4f-47da-a471-e01f481f920e</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>9151915d-f251-4692-84d7-ea02ce8de88f</t>
+    <t>d74cbbe7-bce2-41cb-a1e7-030615c160e1</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>a88f4367-64b4-4fc4-81d3-6bae2fedb33f</t>
+    <t>c78b0791-69f5-42bc-b63f-f7b4d0760623</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>150da03f-88dd-41e6-a8ae-a0f4bc10bd89</t>
+    <t>a0dcba12-834d-4283-b6b3-d4d2f5865553</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>6178d1e7-beea-426f-99a1-005661981f73</t>
+    <t>e3d79e6b-0fc8-4da5-8870-b9de5bb10ab9</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>75448200-00d0-4b37-a05c-fbc21f7aa438</t>
+    <t>d8bc369c-b1d7-4896-b7db-f06fc378a1b7</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>ab94eff3-c57d-4bf4-ab42-4ea07d6cb1af</t>
+    <t>c951266d-ff4a-4999-b2d5-e90ea480dc22</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>f9a8723d-65d6-4492-924f-480d0e1a1cd4</t>
+    <t>6d4da6ff-e948-44e6-bd91-aeed8f5fd1bd</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>dee87e48-2f1b-4389-b62f-574d571dc150</t>
+    <t>83cfaea1-f575-4fbe-a2aa-5ab424114b1d</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>40d6a8d9-9c4c-4006-ac30-53beeb07490a</t>
+    <t>8c0a932e-64c2-4560-9276-d2ab704acebe</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>d1d3b4a9-215b-4ed0-8bee-356a95f4c70d</t>
+    <t>d0fc3004-8671-4c23-bddb-e5afb85fd8ae</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>f8173350-b49e-4dcd-84c5-48b63d4452ec</t>
+    <t>9a41cae6-f435-4faf-926c-97c0013a3463</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>34cbaa8f-86b5-4ae2-b654-d99a2ed3cb5a</t>
+    <t>cf2d9d52-452b-4e3f-a93d-1f65bb6c2b22</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>959425be-8860-44b1-91ac-f4c0253af485</t>
+    <t>03ee0bbd-3d6e-464d-8e07-35ba9aa27f45</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -447,7 +447,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>a169d90a-3a85-405c-b25d-be94fb230eb4</t>
+    <t>dbbc08c5-00c8-4521-9a88-f314894aa1db</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -489,7 +489,7 @@
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>2e978631-2709-4676-9a14-92c77adfed44</t>
+    <t>a072545f-0512-407f-beec-3699544f594b</t>
   </si>
   <si>
     <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
@@ -510,82 +510,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>1152fb02-1ad5-4820-8cfc-86bdc57c064c</t>
-  </si>
-  <si>
-    <t>fcbe639e-1d69-4656-9d89-82df96fac495</t>
-  </si>
-  <si>
-    <t>b2d14700-c63a-4748-8e9a-8dba0c2aefc3</t>
-  </si>
-  <si>
-    <t>b8007a87-13fa-4dd2-bcd0-642edb81b3f4</t>
-  </si>
-  <si>
-    <t>9606f8a2-269a-41fc-a0a4-4f00831367b2</t>
-  </si>
-  <si>
-    <t>877adfaa-bcf0-49bf-8172-d541e35973b6</t>
-  </si>
-  <si>
-    <t>f006df4d-bcd8-4e97-803b-87f791632631</t>
-  </si>
-  <si>
-    <t>a03efa8f-dd43-4ecf-aa38-2205f708e940</t>
-  </si>
-  <si>
-    <t>14862d51-9606-4142-8e69-c3dca46e3ef2</t>
-  </si>
-  <si>
-    <t>52377be3-a7da-428d-b7bc-a8dd2cdcb537</t>
-  </si>
-  <si>
-    <t>a042a9f7-57aa-4a65-85d1-834ea5e7959e</t>
-  </si>
-  <si>
-    <t>133ba07a-8ad7-430c-af6a-7a68a32349dc</t>
-  </si>
-  <si>
-    <t>ff1b30f4-5044-4f4f-bf4b-d749931deeca</t>
-  </si>
-  <si>
-    <t>8f81ebef-e6e8-48e2-9b68-afdbc190d275</t>
-  </si>
-  <si>
-    <t>0f489397-ba05-461f-b7d9-0680d26015dc</t>
-  </si>
-  <si>
-    <t>909470ba-a59c-4723-9bc2-5ec740ddd928</t>
-  </si>
-  <si>
-    <t>2a77e98e-031e-435f-954f-9f9fc83ada32</t>
-  </si>
-  <si>
-    <t>49a5e4e2-b966-4864-85a6-da156adb264a</t>
-  </si>
-  <si>
-    <t>9fa6b9e9-12bd-4c70-b7e7-cf68a47e4d1e</t>
-  </si>
-  <si>
-    <t>ddf5e815-de6b-495f-a024-fc511ef05cbc</t>
-  </si>
-  <si>
-    <t>08e81036-6099-4732-a7c7-ae82806acbdd</t>
-  </si>
-  <si>
-    <t>e548d257-ef90-412b-a236-80bc8eaecb6b</t>
-  </si>
-  <si>
-    <t>c7bd6050-3e1f-499f-8cf2-5a9076e5a3bd</t>
-  </si>
-  <si>
-    <t>8dff710a-e7ff-4d60-9e86-80ca4b753a1d</t>
-  </si>
-  <si>
-    <t>707c9b3a-ce29-497a-b576-defcf429a2b5</t>
-  </si>
-  <si>
-    <t>4555355b-087d-455a-ae7c-4fee8b0d0362</t>
+    <t>d5e407db-4afe-49c8-8aad-eb798ba19a08</t>
+  </si>
+  <si>
+    <t>39c2e1be-8ba7-4b0a-a5db-07fede79f43c</t>
+  </si>
+  <si>
+    <t>d3f48a53-9f07-4528-9c82-e275bc6d6657</t>
+  </si>
+  <si>
+    <t>6f23a2eb-1bc9-456f-b547-6b2d40aa62a4</t>
+  </si>
+  <si>
+    <t>5581f3ad-2c4c-418a-9eef-9bda253b9a64</t>
+  </si>
+  <si>
+    <t>3d28c1a1-70b0-4d68-99a5-39894e3ec3b7</t>
+  </si>
+  <si>
+    <t>1f3fe4cc-9103-4ca5-bcec-3cfa01dc9e9e</t>
+  </si>
+  <si>
+    <t>21676607-d6d3-43a0-a276-1c5129caf46d</t>
+  </si>
+  <si>
+    <t>1d034afd-5f79-4324-9a75-e6c9173ce9b0</t>
+  </si>
+  <si>
+    <t>cc1ac650-6aff-4716-b579-a17b020be526</t>
+  </si>
+  <si>
+    <t>9407f3ff-45ed-4014-801c-068bed7a933d</t>
+  </si>
+  <si>
+    <t>98470116-879f-4a14-813b-8062781f94f3</t>
+  </si>
+  <si>
+    <t>6dd082fc-97a0-4409-bf74-0b172ab6a43d</t>
+  </si>
+  <si>
+    <t>d8a4d705-f704-46fb-91ff-a6911579b00e</t>
+  </si>
+  <si>
+    <t>74855942-e537-4671-82af-24c232b06896</t>
+  </si>
+  <si>
+    <t>9e05542b-5fef-4ea8-ade2-d223d4aef7c4</t>
+  </si>
+  <si>
+    <t>0d613ac9-404b-4da2-84f4-ccb2ea018229</t>
+  </si>
+  <si>
+    <t>812cc5bb-bb0d-49b2-9fe1-7df1e713cc51</t>
+  </si>
+  <si>
+    <t>724f69ad-3467-4cc3-b63f-875973d5293a</t>
+  </si>
+  <si>
+    <t>3708d95f-a8ce-4c2e-9a99-d673d163f3dd</t>
+  </si>
+  <si>
+    <t>43b545da-5c47-407a-a351-a81886e822f5</t>
+  </si>
+  <si>
+    <t>88d0c6ab-c7e7-40d7-b1ba-46a6de1c16cd</t>
+  </si>
+  <si>
+    <t>0fbb45a4-3f65-4f49-8e2d-7b99e404b5c6</t>
+  </si>
+  <si>
+    <t>8341a9c3-fe91-4c8b-b434-3bc03edeee2e</t>
+  </si>
+  <si>
+    <t>e243618c-cf13-4408-ac44-9ec1cf705a96</t>
+  </si>
+  <si>
+    <t>1d4495ac-269f-42a6-b53a-b227021dfd11</t>
   </si>
 </sst>
 </file>

</xml_diff>